<commit_message>
shorten usage of basic initalize and ros run with subprocess
</commit_message>
<xml_diff>
--- a/Greyform-linux-ros1/Python_Application/exporteddatas.xlsx
+++ b/Greyform-linux-ros1/Python_Application/exporteddatas.xlsx
@@ -3563,7 +3563,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -4007,7 +4007,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -6956,7 +6956,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -7061,7 +7061,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finalize listener talker node dialog
finalize listener talker node dialog
</commit_message>
<xml_diff>
--- a/Greyform-linux-ros1/Python_Application/exporteddatas.xlsx
+++ b/Greyform-linux-ros1/Python_Application/exporteddatas.xlsx
@@ -2535,10 +2535,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1474</v>
+        <v>1125</v>
       </c>
       <c r="E2" t="n">
-        <v>2347</v>
+        <v>1125</v>
       </c>
       <c r="F2" t="n">
         <v>1125</v>
@@ -2842,10 +2842,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1878</v>
+        <v>215</v>
       </c>
       <c r="E2" t="n">
-        <v>2290</v>
+        <v>215</v>
       </c>
       <c r="F2" t="n">
         <v>215</v>
@@ -2879,10 +2879,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2351</v>
+        <v>215</v>
       </c>
       <c r="E3" t="n">
-        <v>2290</v>
+        <v>215</v>
       </c>
       <c r="F3" t="n">
         <v>215</v>
@@ -2916,10 +2916,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2633</v>
+        <v>800</v>
       </c>
       <c r="E4" t="n">
-        <v>1785</v>
+        <v>800</v>
       </c>
       <c r="F4" t="n">
         <v>800</v>
@@ -2953,10 +2953,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2833</v>
+        <v>800</v>
       </c>
       <c r="E5" t="n">
-        <v>1785</v>
+        <v>800</v>
       </c>
       <c r="F5" t="n">
         <v>800</v>
@@ -2990,10 +2990,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2833</v>
+        <v>950</v>
       </c>
       <c r="E6" t="n">
-        <v>1785</v>
+        <v>950</v>
       </c>
       <c r="F6" t="n">
         <v>950</v>
@@ -3027,10 +3027,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>978</v>
+        <v>556</v>
       </c>
       <c r="E7" t="n">
-        <v>2045</v>
+        <v>556</v>
       </c>
       <c r="F7" t="n">
         <v>556</v>
@@ -3064,10 +3064,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1021</v>
+        <v>-85</v>
       </c>
       <c r="E8" t="n">
-        <v>2326</v>
+        <v>-85</v>
       </c>
       <c r="F8" t="n">
         <v>-85</v>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -3101,10 +3101,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>978</v>
+        <v>515</v>
       </c>
       <c r="E9" t="n">
-        <v>2369</v>
+        <v>515</v>
       </c>
       <c r="F9" t="n">
         <v>515</v>
@@ -3138,10 +3138,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>903</v>
+        <v>550</v>
       </c>
       <c r="E10" t="n">
-        <v>2385</v>
+        <v>550</v>
       </c>
       <c r="F10" t="n">
         <v>550</v>
@@ -3175,10 +3175,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1053</v>
+        <v>549</v>
       </c>
       <c r="E11" t="n">
-        <v>2385</v>
+        <v>549</v>
       </c>
       <c r="F11" t="n">
         <v>549</v>
@@ -3212,10 +3212,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2513</v>
+        <v>-59</v>
       </c>
       <c r="E12" t="n">
-        <v>1690</v>
+        <v>-59</v>
       </c>
       <c r="F12" t="n">
         <v>-59</v>
@@ -3249,10 +3249,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2513</v>
+        <v>2439</v>
       </c>
       <c r="E13" t="n">
-        <v>1786</v>
+        <v>2439</v>
       </c>
       <c r="F13" t="n">
         <v>2439</v>
@@ -3286,10 +3286,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2753</v>
+        <v>2469</v>
       </c>
       <c r="E14" t="n">
-        <v>1785</v>
+        <v>2469</v>
       </c>
       <c r="F14" t="n">
         <v>2469</v>
@@ -3323,10 +3323,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2753</v>
+        <v>1004</v>
       </c>
       <c r="E15" t="n">
-        <v>1785</v>
+        <v>1004</v>
       </c>
       <c r="F15" t="n">
         <v>1004</v>
@@ -3360,10 +3360,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2513</v>
+        <v>1004</v>
       </c>
       <c r="E16" t="n">
-        <v>1785</v>
+        <v>1004</v>
       </c>
       <c r="F16" t="n">
         <v>1004</v>
@@ -3397,10 +3397,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1563</v>
+        <v>275</v>
       </c>
       <c r="E17" t="n">
-        <v>2385</v>
+        <v>275</v>
       </c>
       <c r="F17" t="n">
         <v>275</v>
@@ -3434,10 +3434,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1513</v>
+        <v>-1775</v>
       </c>
       <c r="E18" t="n">
-        <v>2385</v>
+        <v>-1775</v>
       </c>
       <c r="F18" t="n">
         <v>-1775</v>
@@ -3471,10 +3471,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1513</v>
+        <v>-1747</v>
       </c>
       <c r="E19" t="n">
-        <v>2385</v>
+        <v>-1747</v>
       </c>
       <c r="F19" t="n">
         <v>-1747</v>
@@ -3508,10 +3508,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1053</v>
+        <v>577</v>
       </c>
       <c r="E20" t="n">
-        <v>2385</v>
+        <v>577</v>
       </c>
       <c r="F20" t="n">
         <v>577</v>
@@ -3545,10 +3545,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2833</v>
+        <v>-60</v>
       </c>
       <c r="E21" t="n">
-        <v>1290</v>
+        <v>-60</v>
       </c>
       <c r="F21" t="n">
         <v>-60</v>
@@ -3582,10 +3582,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2633</v>
+        <v>2440</v>
       </c>
       <c r="E22" t="n">
-        <v>1785</v>
+        <v>2440</v>
       </c>
       <c r="F22" t="n">
         <v>2440</v>
@@ -3619,10 +3619,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1303</v>
+        <v>-91</v>
       </c>
       <c r="E23" t="n">
-        <v>2045</v>
+        <v>-91</v>
       </c>
       <c r="F23" t="n">
         <v>-91</v>
@@ -3656,10 +3656,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2289</v>
+        <v>-100</v>
       </c>
       <c r="E24" t="n">
-        <v>1690</v>
+        <v>-100</v>
       </c>
       <c r="F24" t="n">
         <v>-100</v>
@@ -3693,10 +3693,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2203</v>
+        <v>-100</v>
       </c>
       <c r="E25" t="n">
-        <v>1775</v>
+        <v>-100</v>
       </c>
       <c r="F25" t="n">
         <v>-100</v>
@@ -3730,10 +3730,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>598</v>
+        <v>40</v>
       </c>
       <c r="E26" t="n">
-        <v>2170</v>
+        <v>40</v>
       </c>
       <c r="F26" t="n">
         <v>40</v>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -3767,10 +3767,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>678</v>
+        <v>70</v>
       </c>
       <c r="E27" t="n">
-        <v>2090</v>
+        <v>70</v>
       </c>
       <c r="F27" t="n">
         <v>70</v>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -3804,10 +3804,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2138</v>
+        <v>-59</v>
       </c>
       <c r="E28" t="n">
-        <v>1690</v>
+        <v>-59</v>
       </c>
       <c r="F28" t="n">
         <v>-59</v>
@@ -3841,10 +3841,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>903</v>
+        <v>2440</v>
       </c>
       <c r="E29" t="n">
-        <v>2385</v>
+        <v>2440</v>
       </c>
       <c r="F29" t="n">
         <v>2440</v>
@@ -3878,10 +3878,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>903</v>
+        <v>-59</v>
       </c>
       <c r="E30" t="n">
-        <v>2170</v>
+        <v>-59</v>
       </c>
       <c r="F30" t="n">
         <v>-59</v>
@@ -3896,7 +3896,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -3915,10 +3915,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>903</v>
+        <v>-59</v>
       </c>
       <c r="E31" t="n">
-        <v>2199</v>
+        <v>-59</v>
       </c>
       <c r="F31" t="n">
         <v>-59</v>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -3952,10 +3952,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2138</v>
+        <v>40</v>
       </c>
       <c r="E32" t="n">
-        <v>2170</v>
+        <v>40</v>
       </c>
       <c r="F32" t="n">
         <v>40</v>
@@ -3989,10 +3989,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2753</v>
+        <v>-30</v>
       </c>
       <c r="E33" t="n">
-        <v>1590</v>
+        <v>-30</v>
       </c>
       <c r="F33" t="n">
         <v>-30</v>
@@ -4026,10 +4026,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1053</v>
+        <v>2469</v>
       </c>
       <c r="E34" t="n">
-        <v>2385</v>
+        <v>2469</v>
       </c>
       <c r="F34" t="n">
         <v>2469</v>
@@ -4063,10 +4063,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1053</v>
+        <v>-29</v>
       </c>
       <c r="E35" t="n">
-        <v>2090</v>
+        <v>-29</v>
       </c>
       <c r="F35" t="n">
         <v>-29</v>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -4100,10 +4100,10 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1053</v>
+        <v>-29</v>
       </c>
       <c r="E36" t="n">
-        <v>2119</v>
+        <v>-29</v>
       </c>
       <c r="F36" t="n">
         <v>-29</v>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -4137,10 +4137,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1563</v>
+        <v>2469</v>
       </c>
       <c r="E37" t="n">
-        <v>2385</v>
+        <v>2469</v>
       </c>
       <c r="F37" t="n">
         <v>2469</v>
@@ -4174,10 +4174,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1563</v>
+        <v>-29</v>
       </c>
       <c r="E38" t="n">
-        <v>2090</v>
+        <v>-29</v>
       </c>
       <c r="F38" t="n">
         <v>-29</v>
@@ -4211,10 +4211,10 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1563</v>
+        <v>-29</v>
       </c>
       <c r="E39" t="n">
-        <v>2119</v>
+        <v>-29</v>
       </c>
       <c r="F39" t="n">
         <v>-29</v>
@@ -4248,10 +4248,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2058</v>
+        <v>70</v>
       </c>
       <c r="E40" t="n">
-        <v>2090</v>
+        <v>70</v>
       </c>
       <c r="F40" t="n">
         <v>70</v>
@@ -4285,10 +4285,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2058</v>
+        <v>-30</v>
       </c>
       <c r="E41" t="n">
-        <v>1590</v>
+        <v>-30</v>
       </c>
       <c r="F41" t="n">
         <v>-30</v>
@@ -4322,10 +4322,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>678</v>
+        <v>70</v>
       </c>
       <c r="E42" t="n">
-        <v>1445</v>
+        <v>70</v>
       </c>
       <c r="F42" t="n">
         <v>70</v>
@@ -4359,10 +4359,10 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>598</v>
+        <v>39</v>
       </c>
       <c r="E43" t="n">
-        <v>1445</v>
+        <v>39</v>
       </c>
       <c r="F43" t="n">
         <v>39</v>
@@ -4396,10 +4396,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>598</v>
+        <v>190</v>
       </c>
       <c r="E44" t="n">
-        <v>1445</v>
+        <v>190</v>
       </c>
       <c r="F44" t="n">
         <v>190</v>
@@ -4433,10 +4433,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>678</v>
+        <v>189</v>
       </c>
       <c r="E45" t="n">
-        <v>1445</v>
+        <v>189</v>
       </c>
       <c r="F45" t="n">
         <v>189</v>
@@ -4470,10 +4470,10 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>678</v>
+        <v>190</v>
       </c>
       <c r="E46" t="n">
-        <v>1319</v>
+        <v>190</v>
       </c>
       <c r="F46" t="n">
         <v>190</v>
@@ -4507,10 +4507,10 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>708</v>
+        <v>190</v>
       </c>
       <c r="E47" t="n">
-        <v>1319</v>
+        <v>190</v>
       </c>
       <c r="F47" t="n">
         <v>190</v>
@@ -4544,10 +4544,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>758</v>
+        <v>189</v>
       </c>
       <c r="E48" t="n">
-        <v>1319</v>
+        <v>189</v>
       </c>
       <c r="F48" t="n">
         <v>189</v>
@@ -4581,10 +4581,10 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1513</v>
+        <v>90</v>
       </c>
       <c r="E49" t="n">
-        <v>2385</v>
+        <v>90</v>
       </c>
       <c r="F49" t="n">
         <v>90</v>
@@ -4618,10 +4618,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>758</v>
+        <v>189</v>
       </c>
       <c r="E50" t="n">
-        <v>2060</v>
+        <v>189</v>
       </c>
       <c r="F50" t="n">
         <v>189</v>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -4655,10 +4655,10 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1513</v>
+        <v>89</v>
       </c>
       <c r="E51" t="n">
-        <v>2060</v>
+        <v>89</v>
       </c>
       <c r="F51" t="n">
         <v>89</v>
@@ -4692,10 +4692,10 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2679</v>
+        <v>950</v>
       </c>
       <c r="E52" t="n">
-        <v>1747</v>
+        <v>950</v>
       </c>
       <c r="F52" t="n">
         <v>950</v>
@@ -4793,10 +4793,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2241</v>
+        <v>-74</v>
       </c>
       <c r="E2" t="n">
-        <v>2045</v>
+        <v>-74</v>
       </c>
       <c r="F2" t="n">
         <v>-74</v>
@@ -4830,10 +4830,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2618</v>
+        <v>-77</v>
       </c>
       <c r="E3" t="n">
-        <v>1690</v>
+        <v>-77</v>
       </c>
       <c r="F3" t="n">
         <v>-77</v>
@@ -4902,10 +4902,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1924</v>
+        <v>-45</v>
       </c>
       <c r="E5" t="n">
-        <v>2164</v>
+        <v>-45</v>
       </c>
       <c r="F5" t="n">
         <v>-45</v>
@@ -4937,10 +4937,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2327</v>
+        <v>958</v>
       </c>
       <c r="E6" t="n">
-        <v>1376</v>
+        <v>958</v>
       </c>
       <c r="F6" t="n">
         <v>958</v>
@@ -4974,10 +4974,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>574</v>
+        <v>225</v>
       </c>
       <c r="E7" t="n">
-        <v>1797</v>
+        <v>225</v>
       </c>
       <c r="F7" t="n">
         <v>225</v>
@@ -5009,10 +5009,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>749</v>
+        <v>-100</v>
       </c>
       <c r="E8" t="n">
-        <v>722</v>
+        <v>-100</v>
       </c>
       <c r="F8" t="n">
         <v>-100</v>
@@ -5046,10 +5046,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1079</v>
+        <v>-90</v>
       </c>
       <c r="E9" t="n">
-        <v>1052</v>
+        <v>-90</v>
       </c>
       <c r="F9" t="n">
         <v>-90</v>
@@ -5083,10 +5083,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2014</v>
+        <v>1175</v>
       </c>
       <c r="E10" t="n">
-        <v>547</v>
+        <v>1175</v>
       </c>
       <c r="F10" t="n">
         <v>1175</v>
@@ -5120,10 +5120,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2374</v>
+        <v>625</v>
       </c>
       <c r="E11" t="n">
-        <v>1877</v>
+        <v>625</v>
       </c>
       <c r="F11" t="n">
         <v>625</v>
@@ -5155,10 +5155,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1870</v>
+        <v>825</v>
       </c>
       <c r="E12" t="n">
-        <v>1870</v>
+        <v>825</v>
       </c>
       <c r="F12" t="n">
         <v>825</v>
@@ -5190,10 +5190,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>70</v>
+        <v>825</v>
       </c>
       <c r="E13" t="n">
-        <v>1870</v>
+        <v>825</v>
       </c>
       <c r="F13" t="n">
         <v>825</v>
@@ -5225,10 +5225,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1915</v>
+        <v>-25</v>
       </c>
       <c r="E14" t="n">
-        <v>70</v>
+        <v>-25</v>
       </c>
       <c r="F14" t="n">
         <v>-25</v>
@@ -5260,10 +5260,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1905</v>
+        <v>-25</v>
       </c>
       <c r="E15" t="n">
-        <v>70</v>
+        <v>-25</v>
       </c>
       <c r="F15" t="n">
         <v>-25</v>
@@ -5295,10 +5295,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1915</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -5311,7 +5311,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -5330,10 +5330,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1905</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -5365,10 +5365,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1825</v>
+        <v>1175</v>
       </c>
       <c r="E18" t="n">
-        <v>70</v>
+        <v>1175</v>
       </c>
       <c r="F18" t="n">
         <v>1175</v>
@@ -5400,10 +5400,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1245</v>
+        <v>1175</v>
       </c>
       <c r="E19" t="n">
-        <v>70</v>
+        <v>1175</v>
       </c>
       <c r="F19" t="n">
         <v>1175</v>
@@ -5435,10 +5435,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1195</v>
+        <v>1175</v>
       </c>
       <c r="E20" t="n">
-        <v>70</v>
+        <v>1175</v>
       </c>
       <c r="F20" t="n">
         <v>1175</v>
@@ -5470,10 +5470,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1775</v>
+        <v>1175</v>
       </c>
       <c r="E21" t="n">
-        <v>70</v>
+        <v>1175</v>
       </c>
       <c r="F21" t="n">
         <v>1175</v>
@@ -5505,10 +5505,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>70</v>
+        <v>1125</v>
       </c>
       <c r="E22" t="n">
-        <v>1890</v>
+        <v>1125</v>
       </c>
       <c r="F22" t="n">
         <v>1125</v>
@@ -5540,10 +5540,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1870</v>
+        <v>1125</v>
       </c>
       <c r="E23" t="n">
-        <v>1890</v>
+        <v>1125</v>
       </c>
       <c r="F23" t="n">
         <v>1125</v>
@@ -5575,10 +5575,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1277</v>
+        <v>324</v>
       </c>
       <c r="E24" t="n">
-        <v>1870</v>
+        <v>324</v>
       </c>
       <c r="F24" t="n">
         <v>324</v>
@@ -5610,10 +5610,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1242</v>
+        <v>324</v>
       </c>
       <c r="E25" t="n">
-        <v>1870</v>
+        <v>324</v>
       </c>
       <c r="F25" t="n">
         <v>324</v>
@@ -5645,10 +5645,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1597</v>
+        <v>324</v>
       </c>
       <c r="E26" t="n">
-        <v>1870</v>
+        <v>324</v>
       </c>
       <c r="F26" t="n">
         <v>324</v>
@@ -5680,10 +5680,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1562</v>
+        <v>323</v>
       </c>
       <c r="E27" t="n">
-        <v>1870</v>
+        <v>323</v>
       </c>
       <c r="F27" t="n">
         <v>323</v>
@@ -5715,10 +5715,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1055</v>
+        <v>725</v>
       </c>
       <c r="E28" t="n">
-        <v>1890</v>
+        <v>725</v>
       </c>
       <c r="F28" t="n">
         <v>725</v>
@@ -5750,10 +5750,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1182</v>
+        <v>479</v>
       </c>
       <c r="E29" t="n">
-        <v>1890</v>
+        <v>479</v>
       </c>
       <c r="F29" t="n">
         <v>479</v>
@@ -5785,10 +5785,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1182</v>
+        <v>502</v>
       </c>
       <c r="E30" t="n">
-        <v>1890</v>
+        <v>502</v>
       </c>
       <c r="F30" t="n">
         <v>502</v>
@@ -5820,10 +5820,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1182</v>
+        <v>629</v>
       </c>
       <c r="E31" t="n">
-        <v>1890</v>
+        <v>629</v>
       </c>
       <c r="F31" t="n">
         <v>629</v>
@@ -5855,10 +5855,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1182</v>
+        <v>652</v>
       </c>
       <c r="E32" t="n">
-        <v>1890</v>
+        <v>652</v>
       </c>
       <c r="F32" t="n">
         <v>652</v>
@@ -5890,10 +5890,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1659</v>
+        <v>479</v>
       </c>
       <c r="E33" t="n">
-        <v>1890</v>
+        <v>479</v>
       </c>
       <c r="F33" t="n">
         <v>479</v>
@@ -5925,10 +5925,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1659</v>
+        <v>502</v>
       </c>
       <c r="E34" t="n">
-        <v>1890</v>
+        <v>502</v>
       </c>
       <c r="F34" t="n">
         <v>502</v>
@@ -5960,10 +5960,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1659</v>
+        <v>629</v>
       </c>
       <c r="E35" t="n">
-        <v>1890</v>
+        <v>629</v>
       </c>
       <c r="F35" t="n">
         <v>629</v>
@@ -5995,10 +5995,10 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1659</v>
+        <v>652</v>
       </c>
       <c r="E36" t="n">
-        <v>1890</v>
+        <v>652</v>
       </c>
       <c r="F36" t="n">
         <v>652</v>
@@ -6030,10 +6030,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1317</v>
+        <v>-45</v>
       </c>
       <c r="E37" t="n">
-        <v>1729</v>
+        <v>-45</v>
       </c>
       <c r="F37" t="n">
         <v>-45</v>
@@ -6065,10 +6065,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1317</v>
+        <v>-45</v>
       </c>
       <c r="E38" t="n">
-        <v>1695</v>
+        <v>-45</v>
       </c>
       <c r="F38" t="n">
         <v>-45</v>
@@ -6100,10 +6100,10 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1523</v>
+        <v>-45</v>
       </c>
       <c r="E39" t="n">
-        <v>1729</v>
+        <v>-45</v>
       </c>
       <c r="F39" t="n">
         <v>-45</v>
@@ -6135,10 +6135,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1523</v>
+        <v>-45</v>
       </c>
       <c r="E40" t="n">
-        <v>1695</v>
+        <v>-45</v>
       </c>
       <c r="F40" t="n">
         <v>-45</v>
@@ -6170,10 +6170,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1105</v>
+        <v>275</v>
       </c>
       <c r="E41" t="n">
-        <v>1890</v>
+        <v>275</v>
       </c>
       <c r="F41" t="n">
         <v>275</v>
@@ -6205,10 +6205,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1104</v>
+        <v>-29</v>
       </c>
       <c r="E42" t="n">
-        <v>1886</v>
+        <v>-29</v>
       </c>
       <c r="F42" t="n">
         <v>-29</v>
@@ -6240,10 +6240,10 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>595</v>
+        <v>549</v>
       </c>
       <c r="E43" t="n">
-        <v>1890</v>
+        <v>549</v>
       </c>
       <c r="F43" t="n">
         <v>549</v>
@@ -6275,10 +6275,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>577</v>
+        <v>519</v>
       </c>
       <c r="E44" t="n">
-        <v>1890</v>
+        <v>519</v>
       </c>
       <c r="F44" t="n">
         <v>519</v>
@@ -6310,10 +6310,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>445</v>
+        <v>550</v>
       </c>
       <c r="E45" t="n">
-        <v>1890</v>
+        <v>550</v>
       </c>
       <c r="F45" t="n">
         <v>550</v>
@@ -6345,10 +6345,10 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>445</v>
+        <v>40</v>
       </c>
       <c r="E46" t="n">
-        <v>1890</v>
+        <v>40</v>
       </c>
       <c r="F46" t="n">
         <v>40</v>
@@ -6361,7 +6361,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -6380,10 +6380,10 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1870</v>
+        <v>625</v>
       </c>
       <c r="E47" t="n">
-        <v>1359</v>
+        <v>625</v>
       </c>
       <c r="F47" t="n">
         <v>625</v>
@@ -6415,10 +6415,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1870</v>
+        <v>625</v>
       </c>
       <c r="E48" t="n">
-        <v>1309</v>
+        <v>625</v>
       </c>
       <c r="F48" t="n">
         <v>625</v>
@@ -6450,10 +6450,10 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1905</v>
+        <v>-25</v>
       </c>
       <c r="E49" t="n">
-        <v>1270</v>
+        <v>-25</v>
       </c>
       <c r="F49" t="n">
         <v>-25</v>
@@ -6485,10 +6485,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1915</v>
+        <v>-25</v>
       </c>
       <c r="E50" t="n">
-        <v>1270</v>
+        <v>-25</v>
       </c>
       <c r="F50" t="n">
         <v>-25</v>
@@ -6520,10 +6520,10 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1905</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>1270</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -6536,7 +6536,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -6555,10 +6555,10 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>1915</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>1270</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -6571,7 +6571,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -6590,10 +6590,10 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>2105</v>
+        <v>854</v>
       </c>
       <c r="E53" t="n">
-        <v>1270</v>
+        <v>854</v>
       </c>
       <c r="F53" t="n">
         <v>854</v>
@@ -6625,10 +6625,10 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2245</v>
+        <v>854</v>
       </c>
       <c r="E54" t="n">
-        <v>1270</v>
+        <v>854</v>
       </c>
       <c r="F54" t="n">
         <v>854</v>
@@ -6660,10 +6660,10 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>2105</v>
+        <v>1074</v>
       </c>
       <c r="E55" t="n">
-        <v>1270</v>
+        <v>1074</v>
       </c>
       <c r="F55" t="n">
         <v>1074</v>
@@ -6695,10 +6695,10 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>2245</v>
+        <v>1074</v>
       </c>
       <c r="E56" t="n">
-        <v>1270</v>
+        <v>1074</v>
       </c>
       <c r="F56" t="n">
         <v>1074</v>
@@ -6730,10 +6730,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2375</v>
+        <v>-1095</v>
       </c>
       <c r="E57" t="n">
-        <v>1270</v>
+        <v>-1095</v>
       </c>
       <c r="F57" t="n">
         <v>-1095</v>
@@ -6765,10 +6765,10 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>2375</v>
+        <v>-1045</v>
       </c>
       <c r="E58" t="n">
-        <v>1270</v>
+        <v>-1045</v>
       </c>
       <c r="F58" t="n">
         <v>-1045</v>
@@ -6800,10 +6800,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>2375</v>
+        <v>-427</v>
       </c>
       <c r="E59" t="n">
-        <v>1270</v>
+        <v>-427</v>
       </c>
       <c r="F59" t="n">
         <v>-427</v>
@@ -6835,10 +6835,10 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>2375</v>
+        <v>-477</v>
       </c>
       <c r="E60" t="n">
-        <v>1270</v>
+        <v>-477</v>
       </c>
       <c r="F60" t="n">
         <v>-477</v>
@@ -6870,10 +6870,10 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>2182</v>
+        <v>-60</v>
       </c>
       <c r="E61" t="n">
-        <v>1288</v>
+        <v>-60</v>
       </c>
       <c r="F61" t="n">
         <v>-60</v>
@@ -6905,10 +6905,10 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>2375</v>
+        <v>950</v>
       </c>
       <c r="E62" t="n">
-        <v>1290</v>
+        <v>950</v>
       </c>
       <c r="F62" t="n">
         <v>950</v>
@@ -6940,10 +6940,10 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>2630</v>
+        <v>825</v>
       </c>
       <c r="E63" t="n">
-        <v>1290</v>
+        <v>825</v>
       </c>
       <c r="F63" t="n">
         <v>825</v>
@@ -6975,10 +6975,10 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>2055</v>
+        <v>40</v>
       </c>
       <c r="E64" t="n">
-        <v>1290</v>
+        <v>40</v>
       </c>
       <c r="F64" t="n">
         <v>40</v>
@@ -7010,10 +7010,10 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>2294</v>
+        <v>-30</v>
       </c>
       <c r="E65" t="n">
-        <v>1290</v>
+        <v>-30</v>
       </c>
       <c r="F65" t="n">
         <v>-30</v>
@@ -7045,10 +7045,10 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>2850</v>
+        <v>895</v>
       </c>
       <c r="E66" t="n">
-        <v>1149</v>
+        <v>895</v>
       </c>
       <c r="F66" t="n">
         <v>895</v>
@@ -7080,10 +7080,10 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>2210</v>
+        <v>-70</v>
       </c>
       <c r="E67" t="n">
-        <v>1270</v>
+        <v>-70</v>
       </c>
       <c r="F67" t="n">
         <v>-70</v>
@@ -7115,10 +7115,10 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E68" t="n">
-        <v>1270</v>
+        <v>-70</v>
       </c>
       <c r="F68" t="n">
         <v>-70</v>
@@ -7150,10 +7150,10 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E69" t="n">
-        <v>1170</v>
+        <v>-70</v>
       </c>
       <c r="F69" t="n">
         <v>-70</v>
@@ -7185,10 +7185,10 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>2210</v>
+        <v>-70</v>
       </c>
       <c r="E70" t="n">
-        <v>1170</v>
+        <v>-70</v>
       </c>
       <c r="F70" t="n">
         <v>-70</v>
@@ -7220,10 +7220,10 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>1670</v>
+        <v>-45</v>
       </c>
       <c r="E71" t="n">
-        <v>1500</v>
+        <v>-45</v>
       </c>
       <c r="F71" t="n">
         <v>-45</v>
@@ -7255,10 +7255,10 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>1670</v>
+        <v>-45</v>
       </c>
       <c r="E72" t="n">
-        <v>1650</v>
+        <v>-45</v>
       </c>
       <c r="F72" t="n">
         <v>-45</v>
@@ -7290,10 +7290,10 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>1820</v>
+        <v>-45</v>
       </c>
       <c r="E73" t="n">
-        <v>1650</v>
+        <v>-45</v>
       </c>
       <c r="F73" t="n">
         <v>-45</v>
@@ -7325,10 +7325,10 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>1820</v>
+        <v>-45</v>
       </c>
       <c r="E74" t="n">
-        <v>1500</v>
+        <v>-45</v>
       </c>
       <c r="F74" t="n">
         <v>-45</v>
@@ -7360,10 +7360,10 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>2375</v>
+        <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>820</v>
+        <v>0</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -7395,10 +7395,10 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>1450</v>
+        <v>-1172</v>
       </c>
       <c r="E76" t="n">
-        <v>50</v>
+        <v>-1172</v>
       </c>
       <c r="F76" t="n">
         <v>-1172</v>
@@ -7430,10 +7430,10 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>50</v>
+        <v>-1172</v>
       </c>
       <c r="E77" t="n">
-        <v>970</v>
+        <v>-1172</v>
       </c>
       <c r="F77" t="n">
         <v>-1172</v>
@@ -7465,10 +7465,10 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>970</v>
+        <v>-1172</v>
       </c>
       <c r="E78" t="n">
-        <v>1890</v>
+        <v>-1172</v>
       </c>
       <c r="F78" t="n">
         <v>-1172</v>
@@ -7500,10 +7500,10 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>1890</v>
+        <v>-1172</v>
       </c>
       <c r="E79" t="n">
-        <v>1590</v>
+        <v>-1172</v>
       </c>
       <c r="F79" t="n">
         <v>-1172</v>
@@ -7535,10 +7535,10 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>2385</v>
+        <v>-1172</v>
       </c>
       <c r="E80" t="n">
-        <v>1290</v>
+        <v>-1172</v>
       </c>
       <c r="F80" t="n">
         <v>-1172</v>
@@ -7570,10 +7570,10 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>2850</v>
+        <v>-1172</v>
       </c>
       <c r="E81" t="n">
-        <v>670</v>
+        <v>-1172</v>
       </c>
       <c r="F81" t="n">
         <v>-1172</v>
@@ -7605,10 +7605,10 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>1450</v>
+        <v>-45</v>
       </c>
       <c r="E82" t="n">
-        <v>970</v>
+        <v>-45</v>
       </c>
       <c r="F82" t="n">
         <v>-45</v>
@@ -7640,10 +7640,10 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>1451</v>
+        <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>969</v>
+        <v>0</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
@@ -7656,7 +7656,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -7675,10 +7675,10 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>2375</v>
+        <v>225</v>
       </c>
       <c r="E84" t="n">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="F84" t="n">
         <v>225</v>
@@ -7710,10 +7710,10 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>2375</v>
+        <v>825</v>
       </c>
       <c r="E85" t="n">
-        <v>50</v>
+        <v>825</v>
       </c>
       <c r="F85" t="n">
         <v>825</v>
@@ -7745,10 +7745,10 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>2375</v>
+        <v>1425</v>
       </c>
       <c r="E86" t="n">
-        <v>50</v>
+        <v>1425</v>
       </c>
       <c r="F86" t="n">
         <v>1425</v>
@@ -7780,10 +7780,10 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>2375</v>
+        <v>2025</v>
       </c>
       <c r="E87" t="n">
-        <v>50</v>
+        <v>2025</v>
       </c>
       <c r="F87" t="n">
         <v>2025</v>
@@ -7815,10 +7815,10 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>1425</v>
+        <v>225</v>
       </c>
       <c r="E88" t="n">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="F88" t="n">
         <v>225</v>
@@ -7850,10 +7850,10 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>1425</v>
+        <v>825</v>
       </c>
       <c r="E89" t="n">
-        <v>50</v>
+        <v>825</v>
       </c>
       <c r="F89" t="n">
         <v>825</v>
@@ -7888,7 +7888,7 @@
         <v>1425</v>
       </c>
       <c r="E90" t="n">
-        <v>50</v>
+        <v>1425</v>
       </c>
       <c r="F90" t="n">
         <v>1425</v>
@@ -7920,10 +7920,10 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>1425</v>
+        <v>2025</v>
       </c>
       <c r="E91" t="n">
-        <v>50</v>
+        <v>2025</v>
       </c>
       <c r="F91" t="n">
         <v>2025</v>
@@ -7955,10 +7955,10 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>825</v>
+        <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -7990,10 +7990,10 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -8025,10 +8025,10 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>120</v>
+        <v>225</v>
       </c>
       <c r="E94" t="n">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="F94" t="n">
         <v>225</v>
@@ -8060,10 +8060,10 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>120</v>
+        <v>825</v>
       </c>
       <c r="E95" t="n">
-        <v>50</v>
+        <v>825</v>
       </c>
       <c r="F95" t="n">
         <v>825</v>
@@ -8095,10 +8095,10 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>120</v>
+        <v>1425</v>
       </c>
       <c r="E96" t="n">
-        <v>50</v>
+        <v>1425</v>
       </c>
       <c r="F96" t="n">
         <v>1425</v>
@@ -8130,10 +8130,10 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>120</v>
+        <v>2025</v>
       </c>
       <c r="E97" t="n">
-        <v>50</v>
+        <v>2025</v>
       </c>
       <c r="F97" t="n">
         <v>2025</v>
@@ -8165,10 +8165,10 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="E98" t="n">
-        <v>670</v>
+        <v>225</v>
       </c>
       <c r="F98" t="n">
         <v>225</v>
@@ -8200,10 +8200,10 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>50</v>
+        <v>825</v>
       </c>
       <c r="E99" t="n">
-        <v>670</v>
+        <v>825</v>
       </c>
       <c r="F99" t="n">
         <v>825</v>
@@ -8235,10 +8235,10 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>50</v>
+        <v>1425</v>
       </c>
       <c r="E100" t="n">
-        <v>670</v>
+        <v>1425</v>
       </c>
       <c r="F100" t="n">
         <v>1425</v>
@@ -8270,10 +8270,10 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>50</v>
+        <v>2025</v>
       </c>
       <c r="E101" t="n">
-        <v>670</v>
+        <v>2025</v>
       </c>
       <c r="F101" t="n">
         <v>2025</v>
@@ -8305,10 +8305,10 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>50</v>
+        <v>225</v>
       </c>
       <c r="E102" t="n">
-        <v>1270</v>
+        <v>225</v>
       </c>
       <c r="F102" t="n">
         <v>225</v>
@@ -8340,10 +8340,10 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>50</v>
+        <v>825</v>
       </c>
       <c r="E103" t="n">
-        <v>1270</v>
+        <v>825</v>
       </c>
       <c r="F103" t="n">
         <v>825</v>
@@ -8375,10 +8375,10 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>50</v>
+        <v>1425</v>
       </c>
       <c r="E104" t="n">
-        <v>1270</v>
+        <v>1425</v>
       </c>
       <c r="F104" t="n">
         <v>1425</v>
@@ -8410,10 +8410,10 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>50</v>
+        <v>2025</v>
       </c>
       <c r="E105" t="n">
-        <v>1270</v>
+        <v>2025</v>
       </c>
       <c r="F105" t="n">
         <v>2025</v>
@@ -8445,10 +8445,10 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>2850</v>
+        <v>225</v>
       </c>
       <c r="E106" t="n">
-        <v>770</v>
+        <v>225</v>
       </c>
       <c r="F106" t="n">
         <v>225</v>
@@ -8480,10 +8480,10 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>2850</v>
+        <v>825</v>
       </c>
       <c r="E107" t="n">
-        <v>770</v>
+        <v>825</v>
       </c>
       <c r="F107" t="n">
         <v>825</v>
@@ -8515,10 +8515,10 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>2850</v>
+        <v>1425</v>
       </c>
       <c r="E108" t="n">
-        <v>770</v>
+        <v>1425</v>
       </c>
       <c r="F108" t="n">
         <v>1425</v>
@@ -8550,10 +8550,10 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>2850</v>
+        <v>2025</v>
       </c>
       <c r="E109" t="n">
-        <v>770</v>
+        <v>2025</v>
       </c>
       <c r="F109" t="n">
         <v>2025</v>
@@ -8585,10 +8585,10 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>2850</v>
+        <v>225</v>
       </c>
       <c r="E110" t="n">
-        <v>170</v>
+        <v>225</v>
       </c>
       <c r="F110" t="n">
         <v>225</v>
@@ -8620,10 +8620,10 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>2850</v>
+        <v>825</v>
       </c>
       <c r="E111" t="n">
-        <v>170</v>
+        <v>825</v>
       </c>
       <c r="F111" t="n">
         <v>825</v>
@@ -8655,10 +8655,10 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>1890</v>
+        <v>225</v>
       </c>
       <c r="E112" t="n">
-        <v>1650</v>
+        <v>225</v>
       </c>
       <c r="F112" t="n">
         <v>225</v>
@@ -8690,10 +8690,10 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>1890</v>
+        <v>825</v>
       </c>
       <c r="E113" t="n">
-        <v>1870</v>
+        <v>825</v>
       </c>
       <c r="F113" t="n">
         <v>825</v>
@@ -8725,10 +8725,10 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>1890</v>
+        <v>1425</v>
       </c>
       <c r="E114" t="n">
-        <v>1870</v>
+        <v>1425</v>
       </c>
       <c r="F114" t="n">
         <v>1425</v>
@@ -8760,10 +8760,10 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>1890</v>
+        <v>2025</v>
       </c>
       <c r="E115" t="n">
-        <v>1870</v>
+        <v>2025</v>
       </c>
       <c r="F115" t="n">
         <v>2025</v>
@@ -8795,10 +8795,10 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>2375</v>
+        <v>225</v>
       </c>
       <c r="E116" t="n">
-        <v>1290</v>
+        <v>225</v>
       </c>
       <c r="F116" t="n">
         <v>225</v>
@@ -8830,10 +8830,10 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>2375</v>
+        <v>825</v>
       </c>
       <c r="E117" t="n">
-        <v>1290</v>
+        <v>825</v>
       </c>
       <c r="F117" t="n">
         <v>825</v>
@@ -8865,10 +8865,10 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>2375</v>
+        <v>1425</v>
       </c>
       <c r="E118" t="n">
-        <v>1290</v>
+        <v>1425</v>
       </c>
       <c r="F118" t="n">
         <v>1425</v>
@@ -8900,10 +8900,10 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>2375</v>
+        <v>2025</v>
       </c>
       <c r="E119" t="n">
-        <v>1290</v>
+        <v>2025</v>
       </c>
       <c r="F119" t="n">
         <v>2025</v>
@@ -8935,10 +8935,10 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>1890</v>
+        <v>825</v>
       </c>
       <c r="E120" t="n">
-        <v>1650</v>
+        <v>825</v>
       </c>
       <c r="F120" t="n">
         <v>825</v>
@@ -8970,10 +8970,10 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E121" t="n">
-        <v>1670</v>
+        <v>225</v>
       </c>
       <c r="F121" t="n">
         <v>225</v>
@@ -9005,10 +9005,10 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>820</v>
+        <v>225</v>
       </c>
       <c r="E122" t="n">
-        <v>1670</v>
+        <v>225</v>
       </c>
       <c r="F122" t="n">
         <v>225</v>
@@ -9040,10 +9040,10 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>1420</v>
+        <v>225</v>
       </c>
       <c r="E123" t="n">
-        <v>1670</v>
+        <v>225</v>
       </c>
       <c r="F123" t="n">
         <v>225</v>
@@ -9075,10 +9075,10 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>2710</v>
+        <v>-70</v>
       </c>
       <c r="E124" t="n">
-        <v>1119</v>
+        <v>-70</v>
       </c>
       <c r="F124" t="n">
         <v>-70</v>
@@ -9110,10 +9110,10 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>2710</v>
+        <v>-70</v>
       </c>
       <c r="E125" t="n">
-        <v>969</v>
+        <v>-70</v>
       </c>
       <c r="F125" t="n">
         <v>-70</v>
@@ -9145,10 +9145,10 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>2710</v>
+        <v>-70</v>
       </c>
       <c r="E126" t="n">
-        <v>819</v>
+        <v>-70</v>
       </c>
       <c r="F126" t="n">
         <v>-70</v>
@@ -9180,10 +9180,10 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>2710</v>
+        <v>-70</v>
       </c>
       <c r="E127" t="n">
-        <v>670</v>
+        <v>-70</v>
       </c>
       <c r="F127" t="n">
         <v>-70</v>
@@ -9215,10 +9215,10 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>2710</v>
+        <v>-70</v>
       </c>
       <c r="E128" t="n">
-        <v>519</v>
+        <v>-70</v>
       </c>
       <c r="F128" t="n">
         <v>-70</v>
@@ -9250,10 +9250,10 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>2710</v>
+        <v>-70</v>
       </c>
       <c r="E129" t="n">
-        <v>369</v>
+        <v>-70</v>
       </c>
       <c r="F129" t="n">
         <v>-70</v>
@@ -9285,10 +9285,10 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>2710</v>
+        <v>-70</v>
       </c>
       <c r="E130" t="n">
-        <v>219</v>
+        <v>-70</v>
       </c>
       <c r="F130" t="n">
         <v>-70</v>
@@ -9320,10 +9320,10 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E131" t="n">
-        <v>1119</v>
+        <v>-70</v>
       </c>
       <c r="F131" t="n">
         <v>-70</v>
@@ -9355,10 +9355,10 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E132" t="n">
-        <v>969</v>
+        <v>-70</v>
       </c>
       <c r="F132" t="n">
         <v>-70</v>
@@ -9390,10 +9390,10 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E133" t="n">
-        <v>819</v>
+        <v>-70</v>
       </c>
       <c r="F133" t="n">
         <v>-70</v>
@@ -9425,10 +9425,10 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E134" t="n">
-        <v>670</v>
+        <v>-70</v>
       </c>
       <c r="F134" t="n">
         <v>-70</v>
@@ -9460,10 +9460,10 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E135" t="n">
-        <v>519</v>
+        <v>-70</v>
       </c>
       <c r="F135" t="n">
         <v>-70</v>
@@ -9495,10 +9495,10 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E136" t="n">
-        <v>369</v>
+        <v>-70</v>
       </c>
       <c r="F136" t="n">
         <v>-70</v>
@@ -9530,10 +9530,10 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>2110</v>
+        <v>-70</v>
       </c>
       <c r="E137" t="n">
-        <v>219</v>
+        <v>-70</v>
       </c>
       <c r="F137" t="n">
         <v>-70</v>
@@ -9565,10 +9565,10 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>1990</v>
+        <v>110</v>
       </c>
       <c r="E138" t="n">
-        <v>669</v>
+        <v>110</v>
       </c>
       <c r="F138" t="n">
         <v>110</v>
@@ -9600,10 +9600,10 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>1920</v>
+        <v>135</v>
       </c>
       <c r="E139" t="n">
-        <v>669</v>
+        <v>135</v>
       </c>
       <c r="F139" t="n">
         <v>135</v>
@@ -9635,10 +9635,10 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>1420</v>
+        <v>-45</v>
       </c>
       <c r="E140" t="n">
-        <v>1270</v>
+        <v>-45</v>
       </c>
       <c r="F140" t="n">
         <v>-45</v>
@@ -9670,10 +9670,10 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>1420</v>
+        <v>-45</v>
       </c>
       <c r="E141" t="n">
-        <v>670</v>
+        <v>-45</v>
       </c>
       <c r="F141" t="n">
         <v>-45</v>
@@ -9705,10 +9705,10 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>820</v>
+        <v>-45</v>
       </c>
       <c r="E142" t="n">
-        <v>1270</v>
+        <v>-45</v>
       </c>
       <c r="F142" t="n">
         <v>-45</v>
@@ -9740,10 +9740,10 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>820</v>
+        <v>-45</v>
       </c>
       <c r="E143" t="n">
-        <v>670</v>
+        <v>-45</v>
       </c>
       <c r="F143" t="n">
         <v>-45</v>
@@ -9775,10 +9775,10 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>220</v>
+        <v>-45</v>
       </c>
       <c r="E144" t="n">
-        <v>1270</v>
+        <v>-45</v>
       </c>
       <c r="F144" t="n">
         <v>-45</v>
@@ -9810,10 +9810,10 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>220</v>
+        <v>-45</v>
       </c>
       <c r="E145" t="n">
-        <v>670</v>
+        <v>-45</v>
       </c>
       <c r="F145" t="n">
         <v>-45</v>
@@ -9911,10 +9911,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>758</v>
+        <v>189</v>
       </c>
       <c r="E2" t="n">
-        <v>1499</v>
+        <v>189</v>
       </c>
       <c r="F2" t="n">
         <v>189</v>
@@ -9948,10 +9948,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>678</v>
+        <v>90</v>
       </c>
       <c r="E3" t="n">
-        <v>1190</v>
+        <v>90</v>
       </c>
       <c r="F3" t="n">
         <v>90</v>
@@ -9985,10 +9985,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>598</v>
+        <v>89</v>
       </c>
       <c r="E4" t="n">
-        <v>1190</v>
+        <v>89</v>
       </c>
       <c r="F4" t="n">
         <v>89</v>
@@ -10088,10 +10088,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>529</v>
+        <v>-145</v>
       </c>
       <c r="E2" t="n">
-        <v>477</v>
+        <v>-145</v>
       </c>
       <c r="F2" t="n">
         <v>-145</v>
@@ -10125,10 +10125,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>554</v>
+        <v>-145</v>
       </c>
       <c r="E3" t="n">
-        <v>2392</v>
+        <v>-145</v>
       </c>
       <c r="F3" t="n">
         <v>-145</v>
@@ -10143,7 +10143,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -10162,10 +10162,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2419</v>
+        <v>-145</v>
       </c>
       <c r="E4" t="n">
-        <v>2367</v>
+        <v>-145</v>
       </c>
       <c r="F4" t="n">
         <v>-145</v>
@@ -10199,10 +10199,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2444</v>
+        <v>-145</v>
       </c>
       <c r="E5" t="n">
-        <v>1792</v>
+        <v>-145</v>
       </c>
       <c r="F5" t="n">
         <v>-145</v>
@@ -10236,10 +10236,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3379</v>
+        <v>-145</v>
       </c>
       <c r="E6" t="n">
-        <v>1767</v>
+        <v>-145</v>
       </c>
       <c r="F6" t="n">
         <v>-145</v>
@@ -10273,10 +10273,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3354</v>
+        <v>-145</v>
       </c>
       <c r="E7" t="n">
-        <v>502</v>
+        <v>-145</v>
       </c>
       <c r="F7" t="n">
         <v>-145</v>
@@ -10310,10 +10310,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>564</v>
+        <v>-45</v>
       </c>
       <c r="E8" t="n">
-        <v>527</v>
+        <v>-45</v>
       </c>
       <c r="F8" t="n">
         <v>-45</v>
@@ -10345,10 +10345,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2384</v>
+        <v>-45</v>
       </c>
       <c r="E9" t="n">
-        <v>2367</v>
+        <v>-45</v>
       </c>
       <c r="F9" t="n">
         <v>-45</v>
@@ -10380,10 +10380,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2394</v>
+        <v>-70</v>
       </c>
       <c r="E10" t="n">
-        <v>1757</v>
+        <v>-70</v>
       </c>
       <c r="F10" t="n">
         <v>-70</v>
@@ -10415,10 +10415,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3344</v>
+        <v>-70</v>
       </c>
       <c r="E11" t="n">
-        <v>1747</v>
+        <v>-70</v>
       </c>
       <c r="F11" t="n">
         <v>-70</v>
@@ -10450,10 +10450,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2409</v>
+        <v>-45</v>
       </c>
       <c r="E12" t="n">
-        <v>537</v>
+        <v>-45</v>
       </c>
       <c r="F12" t="n">
         <v>-45</v>
@@ -10485,10 +10485,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2414</v>
+        <v>-70</v>
       </c>
       <c r="E13" t="n">
-        <v>537</v>
+        <v>-70</v>
       </c>
       <c r="F13" t="n">
         <v>-70</v>
@@ -10520,10 +10520,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>574</v>
+        <v>825</v>
       </c>
       <c r="E14" t="n">
-        <v>2357</v>
+        <v>825</v>
       </c>
       <c r="F14" t="n">
         <v>825</v>
@@ -10555,10 +10555,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2414</v>
+        <v>-25</v>
       </c>
       <c r="E15" t="n">
-        <v>547</v>
+        <v>-25</v>
       </c>
       <c r="F15" t="n">
         <v>-25</v>
@@ -10790,10 +10790,10 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>245</v>
+        <v>-100</v>
       </c>
       <c r="E6" t="n">
-        <v>245</v>
+        <v>-100</v>
       </c>
       <c r="F6" t="n">
         <v>-100</v>
@@ -10827,10 +10827,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2375</v>
+        <v>60</v>
       </c>
       <c r="E7" t="n">
-        <v>570</v>
+        <v>60</v>
       </c>
       <c r="F7" t="n">
         <v>60</v>
@@ -10864,10 +10864,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>950</v>
+        <v>60</v>
       </c>
       <c r="E8" t="n">
-        <v>970</v>
+        <v>60</v>
       </c>
       <c r="F8" t="n">
         <v>60</v>
@@ -10936,10 +10936,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1767</v>
+        <v>145</v>
       </c>
       <c r="E10" t="n">
-        <v>3379</v>
+        <v>145</v>
       </c>
       <c r="F10" t="n">
         <v>145</v>
@@ -10973,10 +10973,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3354</v>
+        <v>145</v>
       </c>
       <c r="E11" t="n">
-        <v>502</v>
+        <v>145</v>
       </c>
       <c r="F11" t="n">
         <v>145</v>
@@ -11010,10 +11010,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1747</v>
+        <v>70</v>
       </c>
       <c r="E12" t="n">
-        <v>3344</v>
+        <v>70</v>
       </c>
       <c r="F12" t="n">
         <v>70</v>
@@ -11045,10 +11045,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2409</v>
+        <v>45</v>
       </c>
       <c r="E13" t="n">
-        <v>537</v>
+        <v>45</v>
       </c>
       <c r="F13" t="n">
         <v>45</v>
@@ -11080,10 +11080,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>269</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>5</v>
@@ -11327,10 +11327,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>504</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>477</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -11502,10 +11502,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>574</v>
+        <v>-45</v>
       </c>
       <c r="E2" t="n">
-        <v>2127</v>
+        <v>-45</v>
       </c>
       <c r="F2" t="n">
         <v>-45</v>
@@ -11518,7 +11518,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -11603,10 +11603,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2664</v>
+        <v>-50</v>
       </c>
       <c r="E2" t="n">
-        <v>1697</v>
+        <v>-50</v>
       </c>
       <c r="F2" t="n">
         <v>-50</v>
@@ -11638,10 +11638,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2175</v>
+        <v>285</v>
       </c>
       <c r="E3" t="n">
-        <v>2347</v>
+        <v>285</v>
       </c>
       <c r="F3" t="n">
         <v>285</v>
@@ -11654,7 +11654,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>done</t>
         </is>
       </c>
     </row>
@@ -11673,10 +11673,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3038</v>
+        <v>819</v>
       </c>
       <c r="E4" t="n">
-        <v>1748</v>
+        <v>819</v>
       </c>
       <c r="F4" t="n">
         <v>819</v>
@@ -11708,10 +11708,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2249</v>
+        <v>-25</v>
       </c>
       <c r="E5" t="n">
-        <v>2052</v>
+        <v>-25</v>
       </c>
       <c r="F5" t="n">
         <v>-25</v>
@@ -11743,10 +11743,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1609</v>
+        <v>275</v>
       </c>
       <c r="E6" t="n">
-        <v>2127</v>
+        <v>275</v>
       </c>
       <c r="F6" t="n">
         <v>275</v>
@@ -11780,10 +11780,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1924</v>
+        <v>825</v>
       </c>
       <c r="E7" t="n">
-        <v>2238</v>
+        <v>825</v>
       </c>
       <c r="F7" t="n">
         <v>825</v>
@@ -11817,10 +11817,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1024</v>
+        <v>824</v>
       </c>
       <c r="E8" t="n">
-        <v>2287</v>
+        <v>824</v>
       </c>
       <c r="F8" t="n">
         <v>824</v>
@@ -11854,10 +11854,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2049</v>
+        <v>-54</v>
       </c>
       <c r="E9" t="n">
-        <v>2137</v>
+        <v>-54</v>
       </c>
       <c r="F9" t="n">
         <v>-54</v>
@@ -11891,10 +11891,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2879</v>
+        <v>2400</v>
       </c>
       <c r="E10" t="n">
-        <v>1297</v>
+        <v>2400</v>
       </c>
       <c r="F10" t="n">
         <v>2400</v>

</xml_diff>

<commit_message>
excel changes for diameter
</commit_message>
<xml_diff>
--- a/Greyform-linux-ros1/Python_Application/exporteddatas.xlsx
+++ b/Greyform-linux-ros1/Python_Application/exporteddatas.xlsx
@@ -2014,7 +2014,7 @@
         <v>3968</v>
       </c>
       <c r="M3">
-        <v>1440</v>
+        <v>1935</v>
       </c>
       <c r="O3">
         <v>114.4</v>
@@ -2058,7 +2058,7 @@
         <v>1500</v>
       </c>
       <c r="O4">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2096,7 +2096,7 @@
         <v>3968</v>
       </c>
       <c r="M5">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O5">
         <v>20</v>
@@ -2137,7 +2137,7 @@
         <v>3968</v>
       </c>
       <c r="M6">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O6">
         <v>20</v>
@@ -2178,7 +2178,7 @@
         <v>3968</v>
       </c>
       <c r="M7">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O7">
         <v>20</v>
@@ -2219,7 +2219,7 @@
         <v>3968</v>
       </c>
       <c r="M8">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O8">
         <v>20</v>
@@ -2342,7 +2342,7 @@
         <v>3968</v>
       </c>
       <c r="M11">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O11">
         <v>20.4</v>
@@ -2383,7 +2383,7 @@
         <v>3968</v>
       </c>
       <c r="M12">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O12">
         <v>20.4</v>
@@ -2424,7 +2424,7 @@
         <v>3968</v>
       </c>
       <c r="M13">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O13">
         <v>20</v>
@@ -2465,7 +2465,7 @@
         <v>3968</v>
       </c>
       <c r="M14">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O14">
         <v>20</v>
@@ -2506,7 +2506,7 @@
         <v>3968</v>
       </c>
       <c r="M15">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O15">
         <v>20</v>
@@ -2547,7 +2547,7 @@
         <v>3968</v>
       </c>
       <c r="M16">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O16">
         <v>20.4</v>
@@ -2588,7 +2588,7 @@
         <v>3968</v>
       </c>
       <c r="M17">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O17">
         <v>20</v>
@@ -2629,7 +2629,7 @@
         <v>3968</v>
       </c>
       <c r="M18">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O18">
         <v>20</v>
@@ -2752,7 +2752,7 @@
         <v>3968</v>
       </c>
       <c r="M21">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O21">
         <v>25</v>
@@ -2793,7 +2793,7 @@
         <v>3968</v>
       </c>
       <c r="M22">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O22">
         <v>25</v>
@@ -2834,7 +2834,7 @@
         <v>3968</v>
       </c>
       <c r="M23">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O23">
         <v>25</v>
@@ -2875,7 +2875,7 @@
         <v>3968</v>
       </c>
       <c r="M24">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O24">
         <v>25</v>
@@ -2916,7 +2916,7 @@
         <v>3968</v>
       </c>
       <c r="M25">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O25">
         <v>25</v>
@@ -2957,7 +2957,7 @@
         <v>3968</v>
       </c>
       <c r="M26">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O26">
         <v>25</v>
@@ -2998,7 +2998,7 @@
         <v>3968</v>
       </c>
       <c r="M27">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O27">
         <v>20</v>
@@ -3080,7 +3080,7 @@
         <v>3968</v>
       </c>
       <c r="M29">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O29">
         <v>20</v>
@@ -3121,7 +3121,7 @@
         <v>3968</v>
       </c>
       <c r="M30">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O30">
         <v>20</v>
@@ -3162,7 +3162,7 @@
         <v>3968</v>
       </c>
       <c r="M31">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O31">
         <v>20</v>
@@ -3203,7 +3203,7 @@
         <v>3968</v>
       </c>
       <c r="M32">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O32">
         <v>25</v>
@@ -3244,7 +3244,7 @@
         <v>3968</v>
       </c>
       <c r="M33">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O33">
         <v>20</v>
@@ -3285,7 +3285,7 @@
         <v>3968</v>
       </c>
       <c r="M34">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O34">
         <v>20</v>
@@ -3370,7 +3370,7 @@
         <v>1500</v>
       </c>
       <c r="O36">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -3411,7 +3411,7 @@
         <v>1500</v>
       </c>
       <c r="O37">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -3452,7 +3452,7 @@
         <v>1500</v>
       </c>
       <c r="O38">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -3493,7 +3493,7 @@
         <v>1500</v>
       </c>
       <c r="O39">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -3613,7 +3613,7 @@
         <v>3968</v>
       </c>
       <c r="M42">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O42">
         <v>25</v>
@@ -3654,7 +3654,7 @@
         <v>3968</v>
       </c>
       <c r="M43">
-        <v>1935</v>
+        <v>1440</v>
       </c>
       <c r="O43">
         <v>25</v>
@@ -3736,7 +3736,7 @@
         <v>3968</v>
       </c>
       <c r="M45">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O45">
         <v>25</v>
@@ -3777,7 +3777,7 @@
         <v>3968</v>
       </c>
       <c r="M46">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O46">
         <v>20</v>
@@ -3900,7 +3900,7 @@
         <v>3968</v>
       </c>
       <c r="M49">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O49">
         <v>25</v>
@@ -3941,7 +3941,7 @@
         <v>3968</v>
       </c>
       <c r="M50">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O50">
         <v>20</v>
@@ -3982,7 +3982,7 @@
         <v>3968</v>
       </c>
       <c r="M51">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O51">
         <v>20</v>
@@ -4105,7 +4105,7 @@
         <v>3968</v>
       </c>
       <c r="M54">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O54">
         <v>20</v>
@@ -4187,7 +4187,7 @@
         <v>3968</v>
       </c>
       <c r="M56">
-        <v>900</v>
+        <v>2835</v>
       </c>
       <c r="O56">
         <v>20</v>
@@ -4285,7 +4285,7 @@
         <v>3968</v>
       </c>
       <c r="M2">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
   </sheetData>
@@ -6470,7 +6470,7 @@
         <v>3968</v>
       </c>
       <c r="M52">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
   </sheetData>
@@ -6641,7 +6641,7 @@
         <v>3968</v>
       </c>
       <c r="M4">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -6679,7 +6679,7 @@
         <v>3968</v>
       </c>
       <c r="M5">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -6755,7 +6755,7 @@
         <v>3968</v>
       </c>
       <c r="M7">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -6907,7 +6907,7 @@
         <v>3968</v>
       </c>
       <c r="M11">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -6945,7 +6945,7 @@
         <v>3968</v>
       </c>
       <c r="M12">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -6983,7 +6983,7 @@
         <v>3968</v>
       </c>
       <c r="M13">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -7325,7 +7325,7 @@
         <v>3968</v>
       </c>
       <c r="M22">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -7363,7 +7363,7 @@
         <v>3968</v>
       </c>
       <c r="M23">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -7401,7 +7401,7 @@
         <v>3968</v>
       </c>
       <c r="M24">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -7439,7 +7439,7 @@
         <v>3968</v>
       </c>
       <c r="M25">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -7477,7 +7477,7 @@
         <v>3968</v>
       </c>
       <c r="M26">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -7515,7 +7515,7 @@
         <v>3968</v>
       </c>
       <c r="M27">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -7553,7 +7553,7 @@
         <v>3968</v>
       </c>
       <c r="M28">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -7591,7 +7591,7 @@
         <v>3968</v>
       </c>
       <c r="M29">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -7629,7 +7629,7 @@
         <v>3968</v>
       </c>
       <c r="M30">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -7667,7 +7667,7 @@
         <v>3968</v>
       </c>
       <c r="M31">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -7705,7 +7705,7 @@
         <v>3968</v>
       </c>
       <c r="M32">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -7743,7 +7743,7 @@
         <v>3968</v>
       </c>
       <c r="M33">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -7781,7 +7781,7 @@
         <v>3968</v>
       </c>
       <c r="M34">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -7819,7 +7819,7 @@
         <v>3968</v>
       </c>
       <c r="M35">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -7857,7 +7857,7 @@
         <v>3968</v>
       </c>
       <c r="M36">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -8047,7 +8047,7 @@
         <v>3968</v>
       </c>
       <c r="M41">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -8085,7 +8085,7 @@
         <v>3968</v>
       </c>
       <c r="M42">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -8123,7 +8123,7 @@
         <v>3968</v>
       </c>
       <c r="M43">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -8161,7 +8161,7 @@
         <v>3968</v>
       </c>
       <c r="M44">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -8199,7 +8199,7 @@
         <v>3968</v>
       </c>
       <c r="M45">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -8237,7 +8237,7 @@
         <v>3968</v>
       </c>
       <c r="M46">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -8275,7 +8275,7 @@
         <v>3968</v>
       </c>
       <c r="M47">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -8313,7 +8313,7 @@
         <v>3968</v>
       </c>
       <c r="M48">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -8351,7 +8351,7 @@
         <v>3968</v>
       </c>
       <c r="M49">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -8389,7 +8389,7 @@
         <v>3968</v>
       </c>
       <c r="M50">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -8427,7 +8427,7 @@
         <v>3968</v>
       </c>
       <c r="M51">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -8465,7 +8465,7 @@
         <v>3968</v>
       </c>
       <c r="M52">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -8503,7 +8503,7 @@
         <v>3968</v>
       </c>
       <c r="M53">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -8541,7 +8541,7 @@
         <v>3968</v>
       </c>
       <c r="M54">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -8579,7 +8579,7 @@
         <v>3968</v>
       </c>
       <c r="M55">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -8617,7 +8617,7 @@
         <v>3968</v>
       </c>
       <c r="M56">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -8655,7 +8655,7 @@
         <v>3968</v>
       </c>
       <c r="M57">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -8693,7 +8693,7 @@
         <v>3968</v>
       </c>
       <c r="M58">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -8731,7 +8731,7 @@
         <v>3968</v>
       </c>
       <c r="M59">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -8769,7 +8769,7 @@
         <v>3968</v>
       </c>
       <c r="M60">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -8807,7 +8807,7 @@
         <v>3968</v>
       </c>
       <c r="M61">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -8845,7 +8845,7 @@
         <v>3968</v>
       </c>
       <c r="M62">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -8883,7 +8883,7 @@
         <v>3968</v>
       </c>
       <c r="M63">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -8921,7 +8921,7 @@
         <v>3968</v>
       </c>
       <c r="M64">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -8959,7 +8959,7 @@
         <v>3968</v>
       </c>
       <c r="M65">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -9415,7 +9415,7 @@
         <v>3968</v>
       </c>
       <c r="M77">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="78" spans="1:13">
@@ -9453,7 +9453,7 @@
         <v>3968</v>
       </c>
       <c r="M78">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -9491,7 +9491,7 @@
         <v>3968</v>
       </c>
       <c r="M79">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -9529,7 +9529,7 @@
         <v>3968</v>
       </c>
       <c r="M80">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -10213,7 +10213,7 @@
         <v>3968</v>
       </c>
       <c r="M98">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="99" spans="1:13">
@@ -10251,7 +10251,7 @@
         <v>3968</v>
       </c>
       <c r="M99">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="100" spans="1:13">
@@ -10289,7 +10289,7 @@
         <v>3968</v>
       </c>
       <c r="M100">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="101" spans="1:13">
@@ -10327,7 +10327,7 @@
         <v>3968</v>
       </c>
       <c r="M101">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="102" spans="1:13">
@@ -10365,7 +10365,7 @@
         <v>3968</v>
       </c>
       <c r="M102">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="103" spans="1:13">
@@ -10403,7 +10403,7 @@
         <v>3968</v>
       </c>
       <c r="M103">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -10441,7 +10441,7 @@
         <v>3968</v>
       </c>
       <c r="M104">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="105" spans="1:13">
@@ -10479,7 +10479,7 @@
         <v>3968</v>
       </c>
       <c r="M105">
-        <v>2835</v>
+        <v>900</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -10745,7 +10745,7 @@
         <v>3968</v>
       </c>
       <c r="M112">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="113" spans="1:13">
@@ -10783,7 +10783,7 @@
         <v>3968</v>
       </c>
       <c r="M113">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="114" spans="1:13">
@@ -10821,7 +10821,7 @@
         <v>3968</v>
       </c>
       <c r="M114">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="115" spans="1:13">
@@ -10859,7 +10859,7 @@
         <v>3968</v>
       </c>
       <c r="M115">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="116" spans="1:13">
@@ -10897,7 +10897,7 @@
         <v>3968</v>
       </c>
       <c r="M116">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="117" spans="1:13">
@@ -10935,7 +10935,7 @@
         <v>3968</v>
       </c>
       <c r="M117">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="118" spans="1:13">
@@ -10973,7 +10973,7 @@
         <v>3968</v>
       </c>
       <c r="M118">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="119" spans="1:13">
@@ -11011,7 +11011,7 @@
         <v>3968</v>
       </c>
       <c r="M119">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="120" spans="1:13">
@@ -11049,7 +11049,7 @@
         <v>3968</v>
       </c>
       <c r="M120">
-        <v>1440</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="121" spans="1:13">
@@ -11087,7 +11087,7 @@
         <v>3968</v>
       </c>
       <c r="M121">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="122" spans="1:13">
@@ -11125,7 +11125,7 @@
         <v>3968</v>
       </c>
       <c r="M122">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="123" spans="1:13">
@@ -11163,7 +11163,7 @@
         <v>3968</v>
       </c>
       <c r="M123">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="124" spans="1:13">
@@ -13722,7 +13722,7 @@
         <v>3968</v>
       </c>
       <c r="M2">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
   </sheetData>
@@ -13855,7 +13855,7 @@
         <v>3968</v>
       </c>
       <c r="M3">
-        <v>900</v>
+        <v>2835</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -13893,7 +13893,7 @@
         <v>3968</v>
       </c>
       <c r="M4">
-        <v>1935</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="5" spans="1:15">

</xml_diff>